<commit_message>
"Daily Learning and Growing"
</commit_message>
<xml_diff>
--- a/Test Data/APITestData.xlsx
+++ b/Test Data/APITestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Salim\Desktop\Project_2025_Java_TestNG_Cucumber_RestAssured_DB\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE76A285-DFAC-426A-BE20-07B0F21A316D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C85BE1-2A17-4FD5-9730-EB29DEC1124A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6AFB4F1E-DE3D-4DEA-93AD-BE42C0F0F841}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Testcases</t>
   </si>
@@ -39,21 +39,9 @@
     <t>Data3</t>
   </si>
   <si>
-    <t>tc001_Login</t>
-  </si>
-  <si>
     <t>tc002_Purchase</t>
   </si>
   <si>
-    <t>Steve</t>
-  </si>
-  <si>
-    <t>William</t>
-  </si>
-  <si>
-    <t>Henry</t>
-  </si>
-  <si>
     <t>Phone</t>
   </si>
   <si>
@@ -61,6 +49,21 @@
   </si>
   <si>
     <t>Car</t>
+  </si>
+  <si>
+    <t>Data4</t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>tc001_addBook</t>
+  </si>
+  <si>
+    <t>J.K Rowling</t>
+  </si>
+  <si>
+    <t>ISBN:4679-</t>
   </si>
 </sst>
 </file>
@@ -412,18 +415,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE68166A-23EF-4B03-8CB8-929825312B23}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.77734375" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -436,33 +442,39 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>5435</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D3" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>